<commit_message>
I just deleted row 49
</commit_message>
<xml_diff>
--- a/NTV.xlsx
+++ b/NTV.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ADA\Class 2\Gitdemo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF093D41-1BB2-4281-98BC-2E9D50F8DB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-7730" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
   <si>
     <t>Vendor Name</t>
   </si>
@@ -166,9 +172,6 @@
     <t>ChronicCareIQ</t>
   </si>
   <si>
-    <t>Biofourmis</t>
-  </si>
-  <si>
     <t>98point6</t>
   </si>
   <si>
@@ -319,9 +322,6 @@
     <t>Platform specifically designed for chronic care management, including nephrology patients.</t>
   </si>
   <si>
-    <t>AI-driven remote patient monitoring platform that supports nephrology care management.</t>
-  </si>
-  <si>
     <t>Text-based telehealth service with a focus on primary and specialty care, including nephrology.</t>
   </si>
   <si>
@@ -470,9 +470,6 @@
   </si>
   <si>
     <t>https://www.chroniccareiq.com</t>
-  </si>
-  <si>
-    <t>https://www.biofourmis.com</t>
   </si>
   <si>
     <t>https://www.98point6.com</t>
@@ -487,8 +484,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,13 +561,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -608,7 +613,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -642,6 +647,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -676,9 +682,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -851,14 +858,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD49"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -869,620 +878,608 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" t="s">
-        <v>104</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
-    <hyperlink ref="C15" r:id="rId14"/>
-    <hyperlink ref="C16" r:id="rId15"/>
-    <hyperlink ref="C17" r:id="rId16"/>
-    <hyperlink ref="C18" r:id="rId17"/>
-    <hyperlink ref="C19" r:id="rId18"/>
-    <hyperlink ref="C20" r:id="rId19"/>
-    <hyperlink ref="C21" r:id="rId20"/>
-    <hyperlink ref="C22" r:id="rId21"/>
-    <hyperlink ref="C23" r:id="rId22"/>
-    <hyperlink ref="C24" r:id="rId23"/>
-    <hyperlink ref="C25" r:id="rId24"/>
-    <hyperlink ref="C26" r:id="rId25"/>
-    <hyperlink ref="C27" r:id="rId26"/>
-    <hyperlink ref="C28" r:id="rId27"/>
-    <hyperlink ref="C29" r:id="rId28"/>
-    <hyperlink ref="C30" r:id="rId29"/>
-    <hyperlink ref="C31" r:id="rId30"/>
-    <hyperlink ref="C32" r:id="rId31"/>
-    <hyperlink ref="C33" r:id="rId32"/>
-    <hyperlink ref="C34" r:id="rId33"/>
-    <hyperlink ref="C35" r:id="rId34"/>
-    <hyperlink ref="C36" r:id="rId35"/>
-    <hyperlink ref="C37" r:id="rId36"/>
-    <hyperlink ref="C38" r:id="rId37"/>
-    <hyperlink ref="C39" r:id="rId38"/>
-    <hyperlink ref="C40" r:id="rId39"/>
-    <hyperlink ref="C41" r:id="rId40"/>
-    <hyperlink ref="C42" r:id="rId41"/>
-    <hyperlink ref="C43" r:id="rId42"/>
-    <hyperlink ref="C44" r:id="rId43"/>
-    <hyperlink ref="C45" r:id="rId44"/>
-    <hyperlink ref="C46" r:id="rId45"/>
-    <hyperlink ref="C47" r:id="rId46"/>
-    <hyperlink ref="C48" r:id="rId47"/>
-    <hyperlink ref="C49" r:id="rId48"/>
-    <hyperlink ref="C50" r:id="rId49"/>
-    <hyperlink ref="C51" r:id="rId50"/>
-    <hyperlink ref="C52" r:id="rId51"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>